<commit_message>
Added Team Members name
</commit_message>
<xml_diff>
--- a/Our Team.xlsx
+++ b/Our Team.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Miguel\HSHL\3. Drite Semester\Microcontrollers\GitHub01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vickj\Desktop\MicroController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D047762-124A-46AD-A115-3C780A68F948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B0DEF9-D69C-4464-A9FE-D9A8A9D8A228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>First name</t>
   </si>
   <si>
     <t>Second name</t>
+  </si>
+  <si>
+    <t>Abeeb Opeyemi</t>
+  </si>
+  <si>
+    <t>Marwa Mohammed Nabwey</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Nureni</t>
+  </si>
+  <si>
+    <t>Charles Arsenal</t>
+  </si>
+  <si>
+    <t>Okere</t>
+  </si>
+  <si>
+    <t>Amit</t>
+  </si>
+  <si>
+    <t>Chakma</t>
+  </si>
+  <si>
+    <t>Vincent Chinedu</t>
+  </si>
+  <si>
+    <t>Obigwe</t>
+  </si>
+  <si>
+    <t>Miguel Antonio Rodriguez</t>
+  </si>
+  <si>
+    <t>Delgado</t>
   </si>
 </sst>
 </file>
@@ -348,19 +384,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +404,56 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>